<commit_message>
Corrected a typo and added a revision sheet
</commit_message>
<xml_diff>
--- a/lcd decode.xlsx
+++ b/lcd decode.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paul nonadmin\Desktop\Arduino_shield_data\LCD_HT1622_new_version_of_Martys_code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A508D6EE-DE6A-4963-A7E4-F14C7C977799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9523291-6231-4BE0-96DC-865BC1C94CE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="4" xr2:uid="{BF4AB91E-5FF4-40A0-A121-052D5172F618}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{BF4AB91E-5FF4-40A0-A121-052D5172F618}"/>
   </bookViews>
   <sheets>
-    <sheet name="Font HT1622" sheetId="1" r:id="rId1"/>
-    <sheet name="LCD adressing HT1622" sheetId="2" r:id="rId2"/>
-    <sheet name="HT1622 command summary" sheetId="3" r:id="rId3"/>
-    <sheet name="HT1622 LCD timing diagrams" sheetId="4" r:id="rId4"/>
-    <sheet name="LCD add HT1625" sheetId="6" r:id="rId5"/>
+    <sheet name="Revisions" sheetId="7" r:id="rId1"/>
+    <sheet name="Font HT1622" sheetId="1" r:id="rId2"/>
+    <sheet name="LCD adressing HT1622" sheetId="2" r:id="rId3"/>
+    <sheet name="HT1622 command summary" sheetId="3" r:id="rId4"/>
+    <sheet name="HT1622 LCD timing diagrams" sheetId="4" r:id="rId5"/>
+    <sheet name="LCD add HT1625" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="data">'LCD adressing HT1622'!$L$2:$AA$5</definedName>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="233">
   <si>
     <t>bin</t>
   </si>
@@ -631,24 +632,6 @@
     <t>In general:</t>
   </si>
   <si>
-    <t>{Add_H_1,7}</t>
-  </si>
-  <si>
-    <t>{Add_H_1,6}</t>
-  </si>
-  <si>
-    <t>{Add_H_1,3}</t>
-  </si>
-  <si>
-    <t>{Add_H_1,5}</t>
-  </si>
-  <si>
-    <t>{Add_H_1,0}</t>
-  </si>
-  <si>
-    <t>{Add_H_1,8}</t>
-  </si>
-  <si>
     <t>{Add_H_2,D}</t>
   </si>
   <si>
@@ -695,6 +678,69 @@
   </si>
   <si>
     <t>OR in terms of "C"arrays:</t>
+  </si>
+  <si>
+    <t>{Add_L_1,7}</t>
+  </si>
+  <si>
+    <t>{Add_L_1,6}</t>
+  </si>
+  <si>
+    <t>{Add_L_1,3}</t>
+  </si>
+  <si>
+    <t>{Add_L_1,5}</t>
+  </si>
+  <si>
+    <t>{Add_L_1,0}</t>
+  </si>
+  <si>
+    <t>{Add_L_1,8}</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Happymacer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date </t>
+  </si>
+  <si>
+    <t>Revision</t>
+  </si>
+  <si>
+    <t>earlier release</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>pre 2022</t>
+  </si>
+  <si>
+    <t>added HT1625</t>
+  </si>
+  <si>
+    <t>corrected general setup in HT1625 to use ADD_H and ADD_L</t>
+  </si>
+  <si>
+    <t>Github</t>
+  </si>
+  <si>
+    <t>https://github.com/happymacer</t>
+  </si>
+  <si>
+    <t>Youtube</t>
+  </si>
+  <si>
+    <t>Instructables</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MFptCfe7_l4</t>
+  </si>
+  <si>
+    <t>https://www.instructables.com/Lieo-Power-First-PF906-Treadmill-Controller-Circui/</t>
   </si>
 </sst>
 </file>
@@ -705,7 +751,7 @@
     <numFmt numFmtId="164" formatCode="0000"/>
     <numFmt numFmtId="165" formatCode="0000\ 0000\ 0000\ 0000"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -789,6 +835,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1397,7 +1451,7 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1650,6 +1704,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -2530,6 +2611,126 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{823C5D5D-C7DB-403D-9413-52E70F2AED3C}">
+  <dimension ref="A2:C14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="37.5703125" style="113" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="110" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="115" t="s">
+        <v>218</v>
+      </c>
+      <c r="B2" s="113" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="115" t="s">
+        <v>220</v>
+      </c>
+      <c r="B3" s="114">
+        <v>44591</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="115" t="s">
+        <v>227</v>
+      </c>
+      <c r="B4" s="114" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="115" t="s">
+        <v>229</v>
+      </c>
+      <c r="B5" s="114" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="115" t="s">
+        <v>230</v>
+      </c>
+      <c r="B6" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="116" t="s">
+        <v>221</v>
+      </c>
+      <c r="B8" s="117" t="s">
+        <v>223</v>
+      </c>
+      <c r="C8" s="118" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="40">
+        <v>0</v>
+      </c>
+      <c r="B9" s="119" t="s">
+        <v>222</v>
+      </c>
+      <c r="C9" s="120" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="40">
+        <v>1</v>
+      </c>
+      <c r="B10" s="119" t="s">
+        <v>225</v>
+      </c>
+      <c r="C10" s="121">
+        <v>44591</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="40">
+        <v>2</v>
+      </c>
+      <c r="B11" s="119" t="s">
+        <v>226</v>
+      </c>
+      <c r="C11" s="121">
+        <v>44591</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="40"/>
+      <c r="B12" s="119"/>
+      <c r="C12" s="120"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="40"/>
+      <c r="B13" s="119"/>
+      <c r="C13" s="120"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="40"/>
+      <c r="B14" s="119"/>
+      <c r="C14" s="120"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EA4561C-6CDC-42D9-8D4E-1FA80314A565}">
   <dimension ref="A2:Z81"/>
   <sheetViews>
@@ -3504,11 +3705,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6AE2AE5-585E-46C7-A35F-DFF53999FE9F}">
   <dimension ref="B1:AA93"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
@@ -6222,7 +6423,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BE9BD69-3125-4D53-9C74-698F91C9378E}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -6237,7 +6438,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DAB7DC6-C331-48BE-8808-87F7465950F6}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -6252,12 +6453,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80C04644-0D2B-4E3D-9796-4433B568380C}">
   <dimension ref="A1:AC87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O59" sqref="O59"/>
+    <sheetView topLeftCell="L1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AC86" sqref="AC86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7342,7 +7543,7 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B27" s="102" t="str">
         <f>DEC2HEX(C27)</f>
@@ -7439,7 +7640,7 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="B29" s="104" t="str">
         <f t="shared" si="6"/>
@@ -7915,7 +8116,7 @@
     </row>
     <row r="39" spans="1:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="B39" s="108" t="str">
         <f t="shared" si="6"/>
@@ -8039,7 +8240,7 @@
     </row>
     <row r="41" spans="1:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="B41" s="104" t="str">
         <f t="shared" si="6"/>
@@ -8163,7 +8364,7 @@
     </row>
     <row r="43" spans="1:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="B43" s="104" t="str">
         <f t="shared" si="6"/>
@@ -8287,7 +8488,7 @@
     </row>
     <row r="45" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="B45" s="104" t="str">
         <f t="shared" si="6"/>
@@ -8959,7 +9160,7 @@
         <v>1100100  0001</v>
       </c>
       <c r="O56" s="44" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="P56" s="40" t="s">
         <v>2</v>
@@ -8983,7 +9184,7 @@
         <v>7</v>
       </c>
       <c r="W56" s="40" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
     </row>
     <row r="57" spans="3:23" x14ac:dyDescent="0.25">
@@ -9099,7 +9300,7 @@
         <v>1101000  0001</v>
       </c>
       <c r="O58" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="59" spans="3:23" x14ac:dyDescent="0.25">
@@ -9799,78 +10000,78 @@
     </row>
     <row r="86" spans="18:29" x14ac:dyDescent="0.25">
       <c r="R86" s="40" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
       <c r="S86" s="40" t="s">
-        <v>197</v>
+        <v>213</v>
       </c>
       <c r="T86" s="40" t="s">
-        <v>198</v>
+        <v>214</v>
       </c>
       <c r="U86" s="40" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
       <c r="V86" s="40" t="s">
-        <v>197</v>
+        <v>213</v>
       </c>
       <c r="W86" s="40" t="s">
-        <v>199</v>
+        <v>215</v>
       </c>
       <c r="X86" s="40" t="s">
-        <v>199</v>
+        <v>215</v>
       </c>
       <c r="Y86" s="40" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
       <c r="Z86" s="40" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
       <c r="AA86" s="40" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
       <c r="AB86" s="40" t="s">
-        <v>200</v>
+        <v>216</v>
       </c>
       <c r="AC86" s="40" t="s">
-        <v>201</v>
+        <v>217</v>
       </c>
     </row>
     <row r="87" spans="18:29" x14ac:dyDescent="0.25">
       <c r="R87" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="S87" s="40" t="s">
         <v>202</v>
       </c>
-      <c r="S87" s="40" t="s">
-        <v>208</v>
-      </c>
       <c r="T87" s="40" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="U87" s="40" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="V87" s="40" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="W87" s="40" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="X87" s="40" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="Y87" s="40" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="Z87" s="40" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="AA87" s="40" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="AB87" s="40" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="AC87" s="40" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>